<commit_message>
successfully tested on first two test cases
</commit_message>
<xml_diff>
--- a/Validation.xlsx
+++ b/Validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODING\LAWrence-lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29698E1-6CC6-44F5-8FE6-EA2A64B10124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA84F840-8BED-4F5F-B3E7-71780AD49AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4389" yWindow="2166" windowWidth="16589" windowHeight="8502" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="101">
   <si>
     <t>Prompt</t>
   </si>
@@ -398,19 +398,25 @@
     <t xml:space="preserve">Maja Gross kauf sich einen Pullover für CHF 100.-. Nach dem ersten Waschen bemerkt sie, dass sich einige Nähte geöffnet haben. Sie bringt den kaputten Pullover in den Laden zurück. Dort nimmt man den Pullover zurück und die Verkäufern ist bereit Maja Gross einen Gutschein für CHF 100.- auszustellen. Maja Gross möchte aber lieber die CHF 100 in bar zurück und damit etwas anderes machen. </t>
   </si>
   <si>
-    <t>prompt2</t>
-  </si>
-  <si>
-    <t>some prompt here</t>
-  </si>
-  <si>
-    <t>sample prompt here</t>
-  </si>
-  <si>
     <t>gpt-4-1106-preview</t>
   </si>
   <si>
-    <t>gpt-3.5-1106-preview</t>
+    <t>You are a smart and very experienced lawyer in Switzerland. You have a client for whom you need to create an analysis of the legal situation.
+Your task: Based on the situation, the question below, you will create a list of relevant articles and paragraphs that you'll look up. 
+You will always answer in German.
+Your output will always be only a JSON list of relevant law articles along with each relevant paragraph as a JSON in the following structure:
+{{
+    "articles": [
+        {{
+            "article_ref": "OR ART. 27 Abs. 2bis"
+        }}
+        # more articles (if any)
+    ]
+}}
+Legal Situation:
+{situation}
+Legal Question:
+{question}</t>
   </si>
 </sst>
 </file>
@@ -480,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -495,6 +501,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -717,7 +726,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -757,35 +766,22 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="9" t="s">
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
         <v>99</v>
       </c>
-      <c r="C3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" t="s">
-        <v>103</v>
-      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
+      <c r="A4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
error in I/O by column indexes
</commit_message>
<xml_diff>
--- a/Validation.xlsx
+++ b/Validation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODING\LAWrence-lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08021C42-774C-4933-8A1F-4A91373F1BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EF3E31-EF10-4CF8-A317-A39419690647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="108">
   <si>
     <t>Prompt</t>
   </si>
@@ -71,15 +71,6 @@
   </si>
   <si>
     <t>G</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>k</t>
   </si>
   <si>
     <t>L</t>
@@ -419,10 +410,34 @@
     <t>BasePrompt2</t>
   </si>
   <si>
-    <t xml:space="preserve">gpt-4-1106-preview	</t>
+    <t>I</t>
   </si>
   <si>
-    <t>gpt-3.5-turbo-1106</t>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>You are a smart and very experienced lawyer in Switzerland. You have a client for whom you need to create an analysis of the legal situation.
+Your task: Based on the situation, the question below, you will create a list of relevant articles and paragraphs that you'll look up. 
+You will always answer in German.
+Your output will always be only a JSON list of relevant law articles along with each relevant paragraph as a JSON in the following structure:
+{{
+    "articles": [
+        {{
+            "article_ref": "OR ART. 27 Abs. 2bis"
+        }}
+        # more articles (if any)
+    ]
+}}
+Legal Situation:
+{situation}
+Legal Question:
+{question}</t>
+  </si>
+  <si>
+    <t>gpt-4-1106-preview</t>
   </si>
 </sst>
 </file>
@@ -497,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -513,6 +528,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,8 +752,8 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -793,10 +811,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>12</v>
@@ -807,14 +828,14 @@
       <c r="I2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>17</v>
+      <c r="J2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -822,7 +843,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>107</v>
@@ -837,13 +861,13 @@
         <v>14</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -887,25 +911,25 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.7" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -927,10 +951,10 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="8"/>
@@ -953,10 +977,10 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
@@ -979,7 +1003,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -1001,17 +1025,17 @@
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -1031,16 +1055,16 @@
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="8"/>
@@ -1060,19 +1084,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="8"/>
@@ -1093,16 +1117,16 @@
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="8"/>
@@ -1123,19 +1147,19 @@
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -1155,19 +1179,19 @@
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
@@ -1187,19 +1211,19 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D11" s="7">
         <v>2</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
@@ -1219,19 +1243,19 @@
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D12" s="7">
         <v>2</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -1251,19 +1275,19 @@
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D13" s="7">
         <v>2</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
@@ -1283,19 +1307,19 @@
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D14" s="7">
         <v>2</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -1315,16 +1339,16 @@
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D15" s="7">
         <v>2</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
@@ -1345,19 +1369,19 @@
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16" s="7">
         <v>3</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -1377,19 +1401,19 @@
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D17" s="7">
         <v>3</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -1409,19 +1433,19 @@
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D18" s="7">
         <v>3</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -1441,19 +1465,19 @@
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D19" s="7">
         <v>3</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
@@ -1473,19 +1497,19 @@
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D20" s="7">
         <v>3</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
@@ -1505,16 +1529,16 @@
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D21" s="7">
         <v>4</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="8"/>
@@ -1535,19 +1559,19 @@
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D22" s="7">
         <v>5</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
@@ -1567,19 +1591,19 @@
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D23" s="7">
         <v>5</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -1599,19 +1623,19 @@
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D24" s="7">
         <v>5</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
@@ -1631,16 +1655,16 @@
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D25" s="7">
         <v>6</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="8"/>
@@ -1661,19 +1685,19 @@
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D26" s="7">
         <v>7</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
@@ -1693,19 +1717,19 @@
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D27" s="7">
         <v>7</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
@@ -1725,19 +1749,19 @@
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D28" s="7">
         <v>8</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
@@ -1757,16 +1781,16 @@
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D29" s="7">
         <v>8</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="8"/>
@@ -1787,19 +1811,19 @@
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D30" s="7">
         <v>8</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
@@ -1819,19 +1843,19 @@
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D31" s="7">
         <v>8</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
@@ -1851,19 +1875,19 @@
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D32" s="7">
         <v>8</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
@@ -1883,19 +1907,19 @@
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D33" s="7">
         <v>8</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
@@ -1915,16 +1939,16 @@
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D34" s="7">
         <v>9</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="8"/>
@@ -1945,16 +1969,16 @@
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D35" s="7">
         <v>10</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="8"/>

</xml_diff>